<commit_message>
Flow Focusing Q calculator v1.0.0
</commit_message>
<xml_diff>
--- a/DataLog.xlsx
+++ b/DataLog.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:E8"/>
@@ -639,6 +639,22 @@
         <v>1.2</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>test2</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>12</v>
+      </c>
+      <c r="D13" t="n">
+        <v>44</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>